<commit_message>
Refactor Data File Subjects Element
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheet2template.xlsx
+++ b/src/main/resources/spreadsheet2template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15AD183-E6DE-1C4B-A610-0F724E318249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384A80EC-FA47-7147-ADE1-FFF95C287211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8960" yWindow="1100" windowWidth="25600" windowHeight="19560" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>RADx-rad Field Label</t>
   </si>
@@ -138,15 +138,6 @@
   </si>
   <si>
     <t>description_of_project</t>
-  </si>
-  <si>
-    <t>keywords</t>
-  </si>
-  <si>
-    <t>Data File Subjects</t>
-  </si>
-  <si>
-    <t>Subject Identifier</t>
   </si>
   <si>
     <t>Data File Related Resources</t>
@@ -704,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9FA6C8-3052-4F44-924C-F8A85A6A2B10}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,7 +721,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -741,7 +732,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -752,7 +743,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -763,29 +754,29 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>3</v>
@@ -796,18 +787,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>3</v>
@@ -818,7 +809,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>3</v>
@@ -829,7 +820,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>3</v>
@@ -857,7 +848,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -879,7 +870,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -890,7 +881,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -945,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -961,7 +952,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>20</v>
@@ -972,7 +963,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>20</v>
@@ -983,18 +974,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>11</v>
@@ -1011,95 +1002,95 @@
         <v>14</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="B30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>44</v>
+      <c r="B34" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1122,17 +1113,6 @@
       </c>
       <c r="C37" s="9" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>